<commit_message>
modified the ashot jar
</commit_message>
<xml_diff>
--- a/Database/IB/TestData.xlsx
+++ b/Database/IB/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\My_Framework_2020\Workspace\BDD\Database\IB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42ECFC6-FB7E-4FB2-9996-C430A582CB0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2DA576-D27B-4D21-B81E-66C545E324E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="4" r:id="rId1"/>
@@ -768,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1142,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>

</xml_diff>